<commit_message>
Add width to LTS
</commit_message>
<xml_diff>
--- a/pybna/tests/segments.xlsx
+++ b/pybna/tests/segments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\pybna\pybna\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB041F-462F-4836-83C4-8E4D6D1932FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66F9FFB-B2B4-4805-A48E-2EE2522EBD01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38DFA9E7-96FB-498F-83BA-57846E2C1FF4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="16">
   <si>
     <t>buffered_lane</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>low_parking</t>
+  </si>
+  <si>
+    <t>width</t>
   </si>
 </sst>
 </file>
@@ -436,15 +439,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{025BC24C-89F8-40FA-88F7-53E843829534}">
-  <dimension ref="A1:I162"/>
+  <dimension ref="A1:J174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P175" sqref="P175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -464,16 +468,19 @@
         <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -486,14 +493,14 @@
       <c r="F2">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2">
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -506,17 +513,17 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -529,11 +536,11 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -546,14 +553,14 @@
       <c r="F5">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5">
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -566,17 +573,17 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6">
         <v>8</v>
       </c>
-      <c r="I6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -589,11 +596,11 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -606,14 +613,14 @@
       <c r="F8">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8">
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -626,17 +633,17 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9">
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9">
         <v>8</v>
       </c>
-      <c r="I9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -649,11 +656,11 @@
       <c r="F10">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -666,14 +673,14 @@
       <c r="F11">
         <v>2</v>
       </c>
-      <c r="G11" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11">
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -686,17 +693,17 @@
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12">
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>8</v>
       </c>
-      <c r="I12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -709,11 +716,11 @@
       <c r="F13">
         <v>2</v>
       </c>
-      <c r="G13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -726,14 +733,14 @@
       <c r="F14">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14">
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -746,17 +753,17 @@
       <c r="F15">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15">
+      <c r="H15" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15">
         <v>8</v>
       </c>
-      <c r="I15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -769,11 +776,11 @@
       <c r="F16">
         <v>1</v>
       </c>
-      <c r="G16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -786,14 +793,14 @@
       <c r="F17">
         <v>2</v>
       </c>
-      <c r="G17" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17">
+      <c r="H17" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -806,17 +813,17 @@
       <c r="F18">
         <v>2</v>
       </c>
-      <c r="G18" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18">
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18">
         <v>8</v>
       </c>
-      <c r="I18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -829,11 +836,11 @@
       <c r="F19">
         <v>2</v>
       </c>
-      <c r="G19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -846,14 +853,14 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
-        <v>1</v>
-      </c>
-      <c r="H20">
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -866,17 +873,17 @@
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="G21" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21">
+      <c r="H21" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21">
         <v>8</v>
       </c>
-      <c r="I21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -889,11 +896,11 @@
       <c r="F22">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -906,14 +913,14 @@
       <c r="F23">
         <v>2</v>
       </c>
-      <c r="G23" t="s">
-        <v>1</v>
-      </c>
-      <c r="H23">
+      <c r="H23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -926,17 +933,17 @@
       <c r="F24">
         <v>2</v>
       </c>
-      <c r="G24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H24">
+      <c r="H24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24">
         <v>8</v>
       </c>
-      <c r="I24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -949,11 +956,11 @@
       <c r="F25">
         <v>2</v>
       </c>
-      <c r="G25" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
@@ -966,14 +973,14 @@
       <c r="F26">
         <v>1</v>
       </c>
-      <c r="G26" t="s">
-        <v>1</v>
-      </c>
-      <c r="H26">
+      <c r="H26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -986,17 +993,17 @@
       <c r="F27">
         <v>1</v>
       </c>
-      <c r="G27" t="s">
-        <v>1</v>
-      </c>
-      <c r="H27">
+      <c r="H27" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27">
         <v>8</v>
       </c>
-      <c r="I27" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1009,11 +1016,11 @@
       <c r="F28">
         <v>1</v>
       </c>
-      <c r="G28" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -1026,14 +1033,14 @@
       <c r="F29">
         <v>1</v>
       </c>
-      <c r="G29" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29">
+      <c r="H29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1046,17 +1053,17 @@
       <c r="F30">
         <v>1</v>
       </c>
-      <c r="G30" t="s">
-        <v>1</v>
-      </c>
-      <c r="H30">
+      <c r="H30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30">
         <v>8</v>
       </c>
-      <c r="I30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1069,11 +1076,11 @@
       <c r="F31">
         <v>1</v>
       </c>
-      <c r="G31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1086,14 +1093,14 @@
       <c r="F32">
         <v>1</v>
       </c>
-      <c r="G32" t="s">
-        <v>1</v>
-      </c>
-      <c r="H32">
+      <c r="H32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1106,17 +1113,17 @@
       <c r="F33">
         <v>1</v>
       </c>
-      <c r="G33" t="s">
-        <v>1</v>
-      </c>
-      <c r="H33">
+      <c r="H33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>8</v>
       </c>
-      <c r="I33" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>3</v>
       </c>
@@ -1129,11 +1136,11 @@
       <c r="F34">
         <v>1</v>
       </c>
-      <c r="G34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -1146,14 +1153,14 @@
       <c r="F35">
         <v>1</v>
       </c>
-      <c r="G35" t="s">
-        <v>1</v>
-      </c>
-      <c r="H35">
+      <c r="H35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1166,17 +1173,17 @@
       <c r="F36">
         <v>1</v>
       </c>
-      <c r="G36" t="s">
-        <v>1</v>
-      </c>
-      <c r="H36">
+      <c r="H36" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36">
         <v>8</v>
       </c>
-      <c r="I36" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1189,11 +1196,11 @@
       <c r="F37">
         <v>1</v>
       </c>
-      <c r="G37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1206,14 +1213,14 @@
       <c r="F38">
         <v>1</v>
       </c>
-      <c r="G38" t="s">
-        <v>1</v>
-      </c>
-      <c r="H38">
+      <c r="H38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38">
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>3</v>
       </c>
@@ -1226,17 +1233,17 @@
       <c r="F39">
         <v>1</v>
       </c>
-      <c r="G39" t="s">
-        <v>1</v>
-      </c>
-      <c r="H39">
+      <c r="H39" t="s">
+        <v>1</v>
+      </c>
+      <c r="I39">
         <v>8</v>
       </c>
-      <c r="I39" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -1249,11 +1256,11 @@
       <c r="F40">
         <v>1</v>
       </c>
-      <c r="G40" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -1266,14 +1273,14 @@
       <c r="F41">
         <v>1</v>
       </c>
-      <c r="G41" t="s">
-        <v>1</v>
-      </c>
-      <c r="H41">
+      <c r="H41" t="s">
+        <v>1</v>
+      </c>
+      <c r="I41">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>3</v>
       </c>
@@ -1286,17 +1293,17 @@
       <c r="F42">
         <v>1</v>
       </c>
-      <c r="G42" t="s">
-        <v>1</v>
-      </c>
-      <c r="H42">
+      <c r="H42" t="s">
+        <v>1</v>
+      </c>
+      <c r="I42">
         <v>8</v>
       </c>
-      <c r="I42" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -1309,11 +1316,11 @@
       <c r="F43">
         <v>1</v>
       </c>
-      <c r="G43" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
@@ -1326,14 +1333,14 @@
       <c r="F44">
         <v>1</v>
       </c>
-      <c r="G44" t="s">
-        <v>1</v>
-      </c>
-      <c r="H44">
+      <c r="H44" t="s">
+        <v>1</v>
+      </c>
+      <c r="I44">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -1346,17 +1353,17 @@
       <c r="F45">
         <v>1</v>
       </c>
-      <c r="G45" t="s">
-        <v>1</v>
-      </c>
-      <c r="H45">
+      <c r="H45" t="s">
+        <v>1</v>
+      </c>
+      <c r="I45">
         <v>8</v>
       </c>
-      <c r="I45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -1369,11 +1376,11 @@
       <c r="F46">
         <v>1</v>
       </c>
-      <c r="G46" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -1386,14 +1393,14 @@
       <c r="F47">
         <v>1</v>
       </c>
-      <c r="G47" t="s">
-        <v>1</v>
-      </c>
-      <c r="H47">
+      <c r="H47" t="s">
+        <v>1</v>
+      </c>
+      <c r="I47">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>3</v>
       </c>
@@ -1406,17 +1413,17 @@
       <c r="F48">
         <v>1</v>
       </c>
-      <c r="G48" t="s">
-        <v>1</v>
-      </c>
-      <c r="H48">
+      <c r="H48" t="s">
+        <v>1</v>
+      </c>
+      <c r="I48">
         <v>8</v>
       </c>
-      <c r="I48" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -1429,11 +1436,11 @@
       <c r="F49">
         <v>1</v>
       </c>
-      <c r="G49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>3</v>
       </c>
@@ -1446,14 +1453,14 @@
       <c r="F50">
         <v>1</v>
       </c>
-      <c r="G50" t="s">
-        <v>1</v>
-      </c>
-      <c r="H50">
+      <c r="H50" t="s">
+        <v>1</v>
+      </c>
+      <c r="I50">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -1466,17 +1473,17 @@
       <c r="F51">
         <v>1</v>
       </c>
-      <c r="G51" t="s">
-        <v>1</v>
-      </c>
-      <c r="H51">
+      <c r="H51" t="s">
+        <v>1</v>
+      </c>
+      <c r="I51">
         <v>8</v>
       </c>
-      <c r="I51" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -1489,11 +1496,11 @@
       <c r="F52">
         <v>1</v>
       </c>
-      <c r="G52" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -1506,14 +1513,14 @@
       <c r="F53">
         <v>1</v>
       </c>
-      <c r="G53" t="s">
-        <v>1</v>
-      </c>
-      <c r="H53">
+      <c r="H53" t="s">
+        <v>1</v>
+      </c>
+      <c r="I53">
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>3</v>
       </c>
@@ -1526,17 +1533,17 @@
       <c r="F54">
         <v>1</v>
       </c>
-      <c r="G54" t="s">
-        <v>1</v>
-      </c>
-      <c r="H54">
+      <c r="H54" t="s">
+        <v>1</v>
+      </c>
+      <c r="I54">
         <v>8</v>
       </c>
-      <c r="I54" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1549,11 +1556,11 @@
       <c r="F55">
         <v>1</v>
       </c>
-      <c r="G55" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B56">
         <v>40</v>
       </c>
@@ -1566,11 +1573,11 @@
       <c r="F56">
         <v>1</v>
       </c>
-      <c r="G56" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B57">
         <v>40</v>
       </c>
@@ -1583,11 +1590,11 @@
       <c r="F57">
         <v>2</v>
       </c>
-      <c r="G57" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H57" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>40</v>
       </c>
@@ -1600,11 +1607,11 @@
       <c r="F58">
         <v>1</v>
       </c>
-      <c r="G58" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H58" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59">
         <v>40</v>
       </c>
@@ -1617,11 +1624,11 @@
       <c r="F59">
         <v>2</v>
       </c>
-      <c r="G59" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B60">
         <v>40</v>
       </c>
@@ -1634,11 +1641,11 @@
       <c r="F60">
         <v>1</v>
       </c>
-      <c r="G60" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H60" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B61">
         <v>40</v>
       </c>
@@ -1651,11 +1658,11 @@
       <c r="F61">
         <v>2</v>
       </c>
-      <c r="G61" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H61" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B62">
         <v>40</v>
       </c>
@@ -1668,11 +1675,11 @@
       <c r="F62">
         <v>1</v>
       </c>
-      <c r="G62" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H62" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B63">
         <v>40</v>
       </c>
@@ -1685,11 +1692,11 @@
       <c r="F63">
         <v>2</v>
       </c>
-      <c r="G63" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H63" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B64">
         <v>40</v>
       </c>
@@ -1702,11 +1709,11 @@
       <c r="F64">
         <v>1</v>
       </c>
-      <c r="G64" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65">
         <v>40</v>
       </c>
@@ -1719,11 +1726,11 @@
       <c r="F65">
         <v>2</v>
       </c>
-      <c r="G65" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66">
         <v>40</v>
       </c>
@@ -1736,11 +1743,11 @@
       <c r="F66">
         <v>1</v>
       </c>
-      <c r="G66" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67">
         <v>40</v>
       </c>
@@ -1753,11 +1760,11 @@
       <c r="F67">
         <v>2</v>
       </c>
-      <c r="G67" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H67" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68">
         <v>40</v>
       </c>
@@ -1770,11 +1777,11 @@
       <c r="F68">
         <v>1</v>
       </c>
-      <c r="G68" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H68" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69">
         <v>40</v>
       </c>
@@ -1787,11 +1794,11 @@
       <c r="F69">
         <v>2</v>
       </c>
-      <c r="G69" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H69" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70">
         <v>40</v>
       </c>
@@ -1804,11 +1811,11 @@
       <c r="F70">
         <v>1</v>
       </c>
-      <c r="G70" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>40</v>
       </c>
@@ -1821,11 +1828,11 @@
       <c r="F71">
         <v>2</v>
       </c>
-      <c r="G71" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H71" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72">
         <v>40</v>
       </c>
@@ -1838,11 +1845,11 @@
       <c r="F72">
         <v>1</v>
       </c>
-      <c r="G72" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H72" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73">
         <v>40</v>
       </c>
@@ -1855,11 +1862,11 @@
       <c r="F73">
         <v>2</v>
       </c>
-      <c r="G73" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H73" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74">
         <v>35</v>
       </c>
@@ -1872,11 +1879,11 @@
       <c r="F74">
         <v>1</v>
       </c>
-      <c r="G74" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H74" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75">
         <v>35</v>
       </c>
@@ -1889,11 +1896,11 @@
       <c r="F75">
         <v>2</v>
       </c>
-      <c r="G75" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H75" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76">
         <v>35</v>
       </c>
@@ -1906,11 +1913,11 @@
       <c r="F76">
         <v>1</v>
       </c>
-      <c r="G76" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H76" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77">
         <v>35</v>
       </c>
@@ -1923,11 +1930,11 @@
       <c r="F77">
         <v>2</v>
       </c>
-      <c r="G77" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H77" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78">
         <v>35</v>
       </c>
@@ -1940,11 +1947,11 @@
       <c r="F78">
         <v>1</v>
       </c>
-      <c r="G78" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H78" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79">
         <v>35</v>
       </c>
@@ -1957,11 +1964,11 @@
       <c r="F79">
         <v>2</v>
       </c>
-      <c r="G79" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H79" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80">
         <v>35</v>
       </c>
@@ -1974,11 +1981,11 @@
       <c r="F80">
         <v>1</v>
       </c>
-      <c r="G80" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H80" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>35</v>
       </c>
@@ -1991,11 +1998,11 @@
       <c r="F81">
         <v>2</v>
       </c>
-      <c r="G81" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H81" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>35</v>
       </c>
@@ -2008,11 +2015,11 @@
       <c r="F82">
         <v>1</v>
       </c>
-      <c r="G82" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H82" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>35</v>
       </c>
@@ -2025,11 +2032,11 @@
       <c r="F83">
         <v>2</v>
       </c>
-      <c r="G83" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>35</v>
       </c>
@@ -2042,11 +2049,11 @@
       <c r="F84">
         <v>1</v>
       </c>
-      <c r="G84" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>35</v>
       </c>
@@ -2059,11 +2066,11 @@
       <c r="F85">
         <v>2</v>
       </c>
-      <c r="G85" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>35</v>
       </c>
@@ -2076,11 +2083,11 @@
       <c r="F86">
         <v>1</v>
       </c>
-      <c r="G86" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>35</v>
       </c>
@@ -2093,11 +2100,11 @@
       <c r="F87">
         <v>2</v>
       </c>
-      <c r="G87" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>35</v>
       </c>
@@ -2110,11 +2117,11 @@
       <c r="F88">
         <v>1</v>
       </c>
-      <c r="G88" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H88" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>35</v>
       </c>
@@ -2127,11 +2134,11 @@
       <c r="F89">
         <v>2</v>
       </c>
-      <c r="G89" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>35</v>
       </c>
@@ -2144,11 +2151,11 @@
       <c r="F90">
         <v>1</v>
       </c>
-      <c r="G90" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H90" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>35</v>
       </c>
@@ -2161,11 +2168,11 @@
       <c r="F91">
         <v>2</v>
       </c>
-      <c r="G91" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H91" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>30</v>
       </c>
@@ -2178,11 +2185,11 @@
       <c r="F92">
         <v>1</v>
       </c>
-      <c r="G92" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H92" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>30</v>
       </c>
@@ -2195,11 +2202,11 @@
       <c r="F93">
         <v>2</v>
       </c>
-      <c r="G93" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H93" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>30</v>
       </c>
@@ -2212,11 +2219,11 @@
       <c r="F94">
         <v>1</v>
       </c>
-      <c r="G94" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H94" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>30</v>
       </c>
@@ -2229,11 +2236,11 @@
       <c r="F95">
         <v>2</v>
       </c>
-      <c r="G95" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H95" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>30</v>
       </c>
@@ -2246,11 +2253,11 @@
       <c r="F96">
         <v>1</v>
       </c>
-      <c r="G96" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H96" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97">
         <v>30</v>
       </c>
@@ -2263,11 +2270,11 @@
       <c r="F97">
         <v>2</v>
       </c>
-      <c r="G97" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H97" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98">
         <v>30</v>
       </c>
@@ -2280,11 +2287,11 @@
       <c r="F98">
         <v>1</v>
       </c>
-      <c r="G98" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99">
         <v>30</v>
       </c>
@@ -2297,11 +2304,11 @@
       <c r="F99">
         <v>2</v>
       </c>
-      <c r="G99" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H99" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100">
         <v>30</v>
       </c>
@@ -2314,11 +2321,11 @@
       <c r="F100">
         <v>1</v>
       </c>
-      <c r="G100" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H100" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101">
         <v>30</v>
       </c>
@@ -2331,11 +2338,11 @@
       <c r="F101">
         <v>2</v>
       </c>
-      <c r="G101" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H101" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102">
         <v>30</v>
       </c>
@@ -2348,11 +2355,11 @@
       <c r="F102">
         <v>1</v>
       </c>
-      <c r="G102" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H102" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103">
         <v>30</v>
       </c>
@@ -2365,11 +2372,11 @@
       <c r="F103">
         <v>2</v>
       </c>
-      <c r="G103" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H103" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104">
         <v>30</v>
       </c>
@@ -2382,11 +2389,11 @@
       <c r="F104">
         <v>1</v>
       </c>
-      <c r="G104" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H104" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105">
         <v>30</v>
       </c>
@@ -2399,11 +2406,11 @@
       <c r="F105">
         <v>2</v>
       </c>
-      <c r="G105" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H105" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106">
         <v>30</v>
       </c>
@@ -2416,11 +2423,11 @@
       <c r="F106">
         <v>1</v>
       </c>
-      <c r="G106" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H106" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107">
         <v>30</v>
       </c>
@@ -2433,11 +2440,11 @@
       <c r="F107">
         <v>2</v>
       </c>
-      <c r="G107" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H107" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108">
         <v>30</v>
       </c>
@@ -2450,11 +2457,11 @@
       <c r="F108">
         <v>1</v>
       </c>
-      <c r="G108" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H108" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109">
         <v>30</v>
       </c>
@@ -2467,11 +2474,11 @@
       <c r="F109">
         <v>2</v>
       </c>
-      <c r="G109" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H109" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110">
         <v>30</v>
       </c>
@@ -2484,11 +2491,11 @@
       <c r="F110">
         <v>0</v>
       </c>
-      <c r="G110" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H110" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111">
         <v>30</v>
       </c>
@@ -2501,11 +2508,11 @@
       <c r="F111">
         <v>0</v>
       </c>
-      <c r="G111" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H111" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112">
         <v>30</v>
       </c>
@@ -2518,11 +2525,11 @@
       <c r="F112">
         <v>0</v>
       </c>
-      <c r="G112" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H112" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113">
         <v>30</v>
       </c>
@@ -2535,11 +2542,11 @@
       <c r="F113">
         <v>0</v>
       </c>
-      <c r="G113" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H113" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114">
         <v>30</v>
       </c>
@@ -2552,538 +2559,562 @@
       <c r="F114">
         <v>0</v>
       </c>
-      <c r="G114" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H114" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C115" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D115">
+        <v>1</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>26</v>
+      </c>
+      <c r="H115" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <v>30</v>
+      </c>
+      <c r="C116" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <v>26</v>
+      </c>
+      <c r="H116" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B117">
+        <v>30</v>
+      </c>
+      <c r="C117" t="s">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117">
+        <v>18</v>
+      </c>
+      <c r="H117" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B118">
+        <v>30</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>18</v>
+      </c>
+      <c r="H118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>25</v>
+      </c>
+      <c r="C119" t="s">
+        <v>1</v>
+      </c>
+      <c r="D119">
         <v>20001</v>
       </c>
-      <c r="F115">
-        <v>1</v>
-      </c>
-      <c r="G115" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B116">
-        <v>25</v>
-      </c>
-      <c r="C116" t="s">
-        <v>1</v>
-      </c>
-      <c r="D116">
+      <c r="F119">
+        <v>1</v>
+      </c>
+      <c r="H119" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B120">
+        <v>25</v>
+      </c>
+      <c r="C120" t="s">
+        <v>1</v>
+      </c>
+      <c r="D120">
         <v>20001</v>
       </c>
-      <c r="F116">
-        <v>2</v>
-      </c>
-      <c r="G116" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B117">
-        <v>25</v>
-      </c>
-      <c r="C117" t="s">
-        <v>1</v>
-      </c>
-      <c r="D117">
+      <c r="F120">
+        <v>2</v>
+      </c>
+      <c r="H120" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B121">
+        <v>25</v>
+      </c>
+      <c r="C121" t="s">
+        <v>1</v>
+      </c>
+      <c r="D121">
         <v>15001</v>
       </c>
-      <c r="F117">
-        <v>1</v>
-      </c>
-      <c r="G117" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B118">
-        <v>25</v>
-      </c>
-      <c r="C118" t="s">
-        <v>1</v>
-      </c>
-      <c r="D118">
+      <c r="F121">
+        <v>1</v>
+      </c>
+      <c r="H121" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B122">
+        <v>25</v>
+      </c>
+      <c r="C122" t="s">
+        <v>1</v>
+      </c>
+      <c r="D122">
         <v>15001</v>
       </c>
-      <c r="F118">
-        <v>2</v>
-      </c>
-      <c r="G118" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B119">
-        <v>25</v>
-      </c>
-      <c r="C119" t="s">
-        <v>1</v>
-      </c>
-      <c r="D119">
+      <c r="F122">
+        <v>2</v>
+      </c>
+      <c r="H122" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B123">
+        <v>25</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123">
         <v>10001</v>
       </c>
-      <c r="F119">
-        <v>1</v>
-      </c>
-      <c r="G119" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B120">
-        <v>25</v>
-      </c>
-      <c r="C120" t="s">
-        <v>1</v>
-      </c>
-      <c r="D120">
+      <c r="F123">
+        <v>1</v>
+      </c>
+      <c r="H123" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124">
+        <v>25</v>
+      </c>
+      <c r="C124" t="s">
+        <v>1</v>
+      </c>
+      <c r="D124">
         <v>10001</v>
       </c>
-      <c r="F120">
-        <v>2</v>
-      </c>
-      <c r="G120" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B121">
-        <v>25</v>
-      </c>
-      <c r="C121" t="s">
-        <v>1</v>
-      </c>
-      <c r="D121">
+      <c r="F124">
+        <v>2</v>
+      </c>
+      <c r="H124" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125">
+        <v>25</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125">
         <v>5001</v>
       </c>
-      <c r="F121">
-        <v>1</v>
-      </c>
-      <c r="G121" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B122">
-        <v>25</v>
-      </c>
-      <c r="C122" t="s">
-        <v>1</v>
-      </c>
-      <c r="D122">
+      <c r="F125">
+        <v>1</v>
+      </c>
+      <c r="H125" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>25</v>
+      </c>
+      <c r="C126" t="s">
+        <v>1</v>
+      </c>
+      <c r="D126">
         <v>5001</v>
       </c>
-      <c r="F122">
-        <v>2</v>
-      </c>
-      <c r="G122" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B123">
-        <v>25</v>
-      </c>
-      <c r="C123" t="s">
-        <v>1</v>
-      </c>
-      <c r="D123">
+      <c r="F126">
+        <v>2</v>
+      </c>
+      <c r="H126" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>25</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127">
         <v>3001</v>
       </c>
-      <c r="F123">
-        <v>1</v>
-      </c>
-      <c r="G123" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B124">
-        <v>25</v>
-      </c>
-      <c r="C124" t="s">
-        <v>1</v>
-      </c>
-      <c r="D124">
+      <c r="F127">
+        <v>1</v>
+      </c>
+      <c r="H127" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>25</v>
+      </c>
+      <c r="C128" t="s">
+        <v>1</v>
+      </c>
+      <c r="D128">
         <v>3001</v>
       </c>
-      <c r="F124">
-        <v>2</v>
-      </c>
-      <c r="G124" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B125">
-        <v>25</v>
-      </c>
-      <c r="C125" t="s">
-        <v>1</v>
-      </c>
-      <c r="D125">
+      <c r="F128">
+        <v>2</v>
+      </c>
+      <c r="H128" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>25</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1</v>
+      </c>
+      <c r="D129">
         <v>2001</v>
       </c>
-      <c r="F125">
-        <v>1</v>
-      </c>
-      <c r="G125" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B126">
-        <v>25</v>
-      </c>
-      <c r="C126" t="s">
-        <v>1</v>
-      </c>
-      <c r="D126">
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="H129" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130">
+        <v>25</v>
+      </c>
+      <c r="C130" t="s">
+        <v>1</v>
+      </c>
+      <c r="D130">
         <v>2001</v>
       </c>
-      <c r="F126">
-        <v>2</v>
-      </c>
-      <c r="G126" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B127">
-        <v>25</v>
-      </c>
-      <c r="C127" t="s">
-        <v>1</v>
-      </c>
-      <c r="D127">
+      <c r="F130">
+        <v>2</v>
+      </c>
+      <c r="H130" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131">
+        <v>25</v>
+      </c>
+      <c r="C131" t="s">
+        <v>1</v>
+      </c>
+      <c r="D131">
         <v>1001</v>
       </c>
-      <c r="F127">
-        <v>1</v>
-      </c>
-      <c r="G127" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B128">
-        <v>25</v>
-      </c>
-      <c r="C128" t="s">
-        <v>1</v>
-      </c>
-      <c r="D128">
+      <c r="F131">
+        <v>1</v>
+      </c>
+      <c r="H131" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132">
+        <v>25</v>
+      </c>
+      <c r="C132" t="s">
+        <v>1</v>
+      </c>
+      <c r="D132">
         <v>1001</v>
       </c>
-      <c r="F128">
-        <v>2</v>
-      </c>
-      <c r="G128" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B129">
-        <v>25</v>
-      </c>
-      <c r="C129" t="s">
-        <v>1</v>
-      </c>
-      <c r="D129">
+      <c r="F132">
+        <v>2</v>
+      </c>
+      <c r="H132" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133">
+        <v>25</v>
+      </c>
+      <c r="C133" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133">
         <v>501</v>
       </c>
-      <c r="F129">
-        <v>1</v>
-      </c>
-      <c r="G129" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B130">
-        <v>25</v>
-      </c>
-      <c r="C130" t="s">
-        <v>1</v>
-      </c>
-      <c r="D130">
+      <c r="F133">
+        <v>1</v>
+      </c>
+      <c r="H133" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134">
+        <v>25</v>
+      </c>
+      <c r="C134" t="s">
+        <v>1</v>
+      </c>
+      <c r="D134">
         <v>501</v>
       </c>
-      <c r="F130">
-        <v>2</v>
-      </c>
-      <c r="G130" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B131">
-        <v>25</v>
-      </c>
-      <c r="C131" t="s">
-        <v>1</v>
-      </c>
-      <c r="D131">
-        <v>1</v>
-      </c>
-      <c r="F131">
-        <v>1</v>
-      </c>
-      <c r="G131" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B132">
-        <v>25</v>
-      </c>
-      <c r="C132" t="s">
-        <v>1</v>
-      </c>
-      <c r="D132">
-        <v>1</v>
-      </c>
-      <c r="F132">
-        <v>2</v>
-      </c>
-      <c r="G132" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B133">
-        <v>25</v>
-      </c>
-      <c r="C133" t="s">
-        <v>2</v>
-      </c>
-      <c r="D133">
+      <c r="F134">
+        <v>2</v>
+      </c>
+      <c r="H134" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135">
+        <v>25</v>
+      </c>
+      <c r="C135" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
+      <c r="H135" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136">
+        <v>25</v>
+      </c>
+      <c r="C136" t="s">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="F136">
+        <v>2</v>
+      </c>
+      <c r="H136" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>25</v>
+      </c>
+      <c r="C137" t="s">
+        <v>2</v>
+      </c>
+      <c r="D137">
         <v>3001</v>
       </c>
-      <c r="F133">
-        <v>0</v>
-      </c>
-      <c r="G133" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B134">
-        <v>25</v>
-      </c>
-      <c r="C134" t="s">
-        <v>2</v>
-      </c>
-      <c r="D134">
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="H137" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138">
+        <v>25</v>
+      </c>
+      <c r="C138" t="s">
+        <v>2</v>
+      </c>
+      <c r="D138">
         <v>2001</v>
       </c>
-      <c r="F134">
-        <v>0</v>
-      </c>
-      <c r="G134" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B135">
-        <v>25</v>
-      </c>
-      <c r="C135" t="s">
-        <v>2</v>
-      </c>
-      <c r="D135">
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="H138" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139">
+        <v>25</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2</v>
+      </c>
+      <c r="D139">
         <v>1001</v>
       </c>
-      <c r="F135">
-        <v>0</v>
-      </c>
-      <c r="G135" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B136">
-        <v>25</v>
-      </c>
-      <c r="C136" t="s">
-        <v>2</v>
-      </c>
-      <c r="D136">
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="H139" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140">
+        <v>25</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+      <c r="D140">
         <v>501</v>
       </c>
-      <c r="F136">
-        <v>0</v>
-      </c>
-      <c r="G136" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B137">
-        <v>25</v>
-      </c>
-      <c r="C137" t="s">
-        <v>2</v>
-      </c>
-      <c r="D137">
-        <v>1</v>
-      </c>
-      <c r="F137">
-        <v>0</v>
-      </c>
-      <c r="G137" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B138">
-        <v>20</v>
-      </c>
-      <c r="C138" t="s">
-        <v>1</v>
-      </c>
-      <c r="D138">
-        <v>20001</v>
-      </c>
-      <c r="F138">
-        <v>1</v>
-      </c>
-      <c r="G138" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B139">
-        <v>20</v>
-      </c>
-      <c r="C139" t="s">
-        <v>1</v>
-      </c>
-      <c r="D139">
-        <v>20001</v>
-      </c>
-      <c r="F139">
-        <v>2</v>
-      </c>
-      <c r="G139" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B140">
-        <v>20</v>
-      </c>
-      <c r="C140" t="s">
-        <v>1</v>
-      </c>
-      <c r="D140">
-        <v>15001</v>
-      </c>
       <c r="F140">
-        <v>1</v>
-      </c>
-      <c r="G140" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H140" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C141" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D141">
-        <v>15001</v>
+        <v>1</v>
       </c>
       <c r="F141">
-        <v>2</v>
-      </c>
-      <c r="G141" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H141" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C142" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D142">
-        <v>10001</v>
+        <v>1</v>
       </c>
       <c r="F142">
-        <v>1</v>
-      </c>
-      <c r="G142" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G142">
+        <v>26</v>
+      </c>
+      <c r="H142" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C143" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D143">
-        <v>10001</v>
+        <v>1</v>
       </c>
       <c r="F143">
-        <v>2</v>
-      </c>
-      <c r="G143" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G143">
+        <v>26</v>
+      </c>
+      <c r="H143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C144" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D144">
-        <v>5001</v>
+        <v>1</v>
       </c>
       <c r="F144">
-        <v>1</v>
-      </c>
-      <c r="G144" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G144">
+        <v>18</v>
+      </c>
+      <c r="H144" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C145" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D145">
-        <v>5001</v>
+        <v>1</v>
       </c>
       <c r="F145">
-        <v>2</v>
-      </c>
-      <c r="G145" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G145">
+        <v>18</v>
+      </c>
+      <c r="H145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B146">
         <v>20</v>
       </c>
@@ -3091,16 +3122,16 @@
         <v>1</v>
       </c>
       <c r="D146">
-        <v>3001</v>
+        <v>20001</v>
       </c>
       <c r="F146">
         <v>1</v>
       </c>
-      <c r="G146" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H146" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B147">
         <v>20</v>
       </c>
@@ -3108,16 +3139,16 @@
         <v>1</v>
       </c>
       <c r="D147">
-        <v>3001</v>
+        <v>20001</v>
       </c>
       <c r="F147">
         <v>2</v>
       </c>
-      <c r="G147" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H147" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148">
         <v>20</v>
       </c>
@@ -3125,16 +3156,16 @@
         <v>1</v>
       </c>
       <c r="D148">
-        <v>2001</v>
+        <v>15001</v>
       </c>
       <c r="F148">
         <v>1</v>
       </c>
-      <c r="G148" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H148" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149">
         <v>20</v>
       </c>
@@ -3142,16 +3173,16 @@
         <v>1</v>
       </c>
       <c r="D149">
-        <v>2001</v>
+        <v>15001</v>
       </c>
       <c r="F149">
         <v>2</v>
       </c>
-      <c r="G149" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H149" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150">
         <v>20</v>
       </c>
@@ -3159,16 +3190,16 @@
         <v>1</v>
       </c>
       <c r="D150">
-        <v>1001</v>
+        <v>10001</v>
       </c>
       <c r="F150">
         <v>1</v>
       </c>
-      <c r="G150" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H150" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151">
         <v>20</v>
       </c>
@@ -3176,16 +3207,16 @@
         <v>1</v>
       </c>
       <c r="D151">
-        <v>1001</v>
+        <v>10001</v>
       </c>
       <c r="F151">
         <v>2</v>
       </c>
-      <c r="G151" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H151" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152">
         <v>20</v>
       </c>
@@ -3193,16 +3224,16 @@
         <v>1</v>
       </c>
       <c r="D152">
-        <v>501</v>
+        <v>5001</v>
       </c>
       <c r="F152">
         <v>1</v>
       </c>
-      <c r="G152" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H152" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153">
         <v>20</v>
       </c>
@@ -3210,16 +3241,16 @@
         <v>1</v>
       </c>
       <c r="D153">
-        <v>501</v>
+        <v>5001</v>
       </c>
       <c r="F153">
         <v>2</v>
       </c>
-      <c r="G153" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H153" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154">
         <v>20</v>
       </c>
@@ -3227,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="D154">
-        <v>1</v>
+        <v>3001</v>
       </c>
       <c r="F154">
         <v>1</v>
       </c>
-      <c r="G154" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H154" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B155">
         <v>20</v>
       </c>
@@ -3244,107 +3275,323 @@
         <v>1</v>
       </c>
       <c r="D155">
-        <v>1</v>
+        <v>3001</v>
       </c>
       <c r="F155">
         <v>2</v>
       </c>
-      <c r="G155" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H155" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B156">
         <v>20</v>
       </c>
       <c r="C156" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D156">
-        <v>3001</v>
+        <v>2001</v>
       </c>
       <c r="F156">
-        <v>0</v>
-      </c>
-      <c r="G156" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H156" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B157">
         <v>20</v>
       </c>
       <c r="C157" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D157">
         <v>2001</v>
       </c>
       <c r="F157">
-        <v>0</v>
-      </c>
-      <c r="G157" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H157" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B158">
         <v>20</v>
       </c>
       <c r="C158" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D158">
         <v>1001</v>
       </c>
       <c r="F158">
-        <v>0</v>
-      </c>
-      <c r="G158" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H158" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B159">
         <v>20</v>
       </c>
       <c r="C159" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D159">
-        <v>501</v>
+        <v>1001</v>
       </c>
       <c r="F159">
-        <v>0</v>
-      </c>
-      <c r="G159" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="H159" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B160">
         <v>20</v>
       </c>
       <c r="C160" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D160">
-        <v>1</v>
+        <v>501</v>
       </c>
       <c r="F160">
-        <v>0</v>
-      </c>
-      <c r="G160" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+        <v>1</v>
+      </c>
+      <c r="H160" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B161">
+        <v>20</v>
+      </c>
+      <c r="C161" t="s">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>501</v>
+      </c>
+      <c r="F161">
+        <v>2</v>
+      </c>
+      <c r="H161" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B162">
+        <v>20</v>
+      </c>
+      <c r="C162" t="s">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <v>1</v>
+      </c>
+      <c r="H162" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B163">
+        <v>20</v>
+      </c>
+      <c r="C163" t="s">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <v>2</v>
+      </c>
+      <c r="H163" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B164">
+        <v>20</v>
+      </c>
+      <c r="C164" t="s">
+        <v>2</v>
+      </c>
+      <c r="D164">
+        <v>3001</v>
+      </c>
+      <c r="F164">
+        <v>0</v>
+      </c>
+      <c r="H164" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B165">
+        <v>20</v>
+      </c>
+      <c r="C165" t="s">
+        <v>2</v>
+      </c>
+      <c r="D165">
+        <v>2001</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="H165" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B166">
+        <v>20</v>
+      </c>
+      <c r="C166" t="s">
+        <v>2</v>
+      </c>
+      <c r="D166">
+        <v>1001</v>
+      </c>
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="H166" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B167">
+        <v>20</v>
+      </c>
+      <c r="C167" t="s">
+        <v>2</v>
+      </c>
+      <c r="D167">
+        <v>501</v>
+      </c>
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="H167" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B168">
+        <v>20</v>
+      </c>
+      <c r="C168" t="s">
+        <v>2</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>0</v>
+      </c>
+      <c r="H168" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B169">
+        <v>20</v>
+      </c>
+      <c r="C169" t="s">
+        <v>2</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+      <c r="G169">
+        <v>26</v>
+      </c>
+      <c r="H169" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B170">
+        <v>20</v>
+      </c>
+      <c r="C170" t="s">
+        <v>2</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+      <c r="G170">
+        <v>26</v>
+      </c>
+      <c r="H170" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B171">
+        <v>20</v>
+      </c>
+      <c r="C171" t="s">
+        <v>2</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+      <c r="G171">
+        <v>18</v>
+      </c>
+      <c r="H171" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B172">
+        <v>20</v>
+      </c>
+      <c r="C172" t="s">
+        <v>2</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="G172">
+        <v>18</v>
+      </c>
+      <c r="H172" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>